<commit_message>
Updated for Loinc and otehrs
</commit_message>
<xml_diff>
--- a/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
+++ b/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subracr1/Projects/tanagra/tanagra-workbench/api/db-cdr/generate-cdr/cb-criteria-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A080344-4B50-9640-827C-24C7BE2EA0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33919471-3E34-0B4A-BFE4-C79C2AA7358A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="34660" windowHeight="19080" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1300" windowWidth="34660" windowHeight="19080" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-CPT4" sheetId="2" r:id="rId1"/>
@@ -22,13 +22,18 @@
     <sheet name="07-DEMOGRAPHICS" sheetId="13" r:id="rId7"/>
     <sheet name="08-VISIT-OCCURRENCE" sheetId="14" r:id="rId8"/>
     <sheet name="09-ICD9" sheetId="1" r:id="rId9"/>
+    <sheet name="10-ICD10CM" sheetId="16" r:id="rId10"/>
+    <sheet name="11-ICD10PCS" sheetId="18" r:id="rId11"/>
+    <sheet name="12-SNOMED-SOURCE" sheetId="19" r:id="rId12"/>
+    <sheet name="13-SNOMED-STANDARD" sheetId="20" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1988" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2219" uniqueCount="161">
   <si>
     <t>run_type</t>
   </si>
@@ -645,6 +650,173 @@
   <si>
     <t>Pharmacy visit</t>
   </si>
+  <si>
+    <t>ICD10CM</t>
+  </si>
+  <si>
+    <t>icd10-name</t>
+  </si>
+  <si>
+    <t>4955215*</t>
+  </si>
+  <si>
+    <t>66223*</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- ICD10CM SOURCE - SQL-ORDER = 10
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'CONDITION' and type = 'ICD10CM' group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'CONDITION' and type = 'ICD10CM' group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'CONDITION' and type = 'ICD10CM' group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'CONDITION' and type = 'ICD10CM' group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'CONDITION' and type = 'ICD10CM' group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- ICD10PCS SOURCE - SQL-ORDER = 11
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'PROCEDURE' and type = 'ICD10PCS' group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'PROCEDURE' and type = 'ICD10PCS' group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'PROCEDURE' and type = 'ICD10PCS' group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'PROCEDURE' and type = 'ICD10PCS' group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'icd10-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'PROCEDURE' and type = 'ICD10PCS' group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>ICD10PCS</t>
+  </si>
+  <si>
+    <t>276159*</t>
+  </si>
+  <si>
+    <t>295*</t>
+  </si>
+  <si>
+    <t>209696*</t>
+  </si>
+  <si>
+    <t>17931*</t>
+  </si>
+  <si>
+    <t>SNOMED</t>
+  </si>
+  <si>
+    <t>31028239*</t>
+  </si>
+  <si>
+    <t>809717*</t>
+  </si>
+  <si>
+    <t>snomed-src-name</t>
+  </si>
+  <si>
+    <t>686674*</t>
+  </si>
+  <si>
+    <t>31853052*</t>
+  </si>
+  <si>
+    <t>177834008*</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- CONDITION_OCCURRENCE - SNOMED - SOURCE - SQL-ORDER = 12
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group,  'snomed-src-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 0 group by 5,4,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group,  'snomed-src-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 0 group by 5,4,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group,  'snomed-src-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 0 group by 5,4,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group,  'snomed-src-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 0 group by 5,4,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group,  'snomed-src-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 0 group by 5,4,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- CONDITION_OCCURRENCE - SNOMED - STANDARD - SQL-ORDER = 13
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'snomed-std-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'CONDITION' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>snomed-std-name</t>
+  </si>
+  <si>
+    <t>1024974*</t>
+  </si>
+  <si>
+    <t>23372658*</t>
+  </si>
+  <si>
+    <t>37830479*</t>
+  </si>
+  <si>
+    <t>153328729*</t>
+  </si>
 </sst>
 </file>
 
@@ -1204,7 +1376,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1278,6 +1450,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1637,7 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE4D1F7-1319-6C48-8687-6B9A4CD5EB11}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2423,11 +2598,3383 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB06DA13-6484-E046-88B0-72C4B033A9D4}">
+  <dimension ref="A1:Z28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="11"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="3">
+        <v>20187</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="L2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="3">
+        <v>20187</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20187</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20187</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2695033</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="29">
+        <v>20187</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2695033</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2695033</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="4">
+        <v>11776</v>
+      </c>
+      <c r="G7" s="4">
+        <v>66245</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="4">
+        <v>11776</v>
+      </c>
+      <c r="G8" s="4">
+        <v>66245</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="4">
+        <v>11776</v>
+      </c>
+      <c r="G9" s="4">
+        <v>66245</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="I9" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11776</v>
+      </c>
+      <c r="G10" s="4">
+        <v>66245</v>
+      </c>
+      <c r="H10" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="I10" s="4">
+        <v>4955237</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="29">
+        <v>11776</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="15"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="15"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="15"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="15"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="16"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="15"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="15"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="15"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="15"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="16"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B20E09-DDDF-534D-930E-DC23CD14C7EF}">
+  <dimension ref="A1:Z28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="11"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="3">
+        <v>7569</v>
+      </c>
+      <c r="G2" s="3">
+        <v>64520</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>64520</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="L2" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="3">
+        <v>7569</v>
+      </c>
+      <c r="G3" s="3">
+        <v>64520</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>64520</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="3">
+        <v>7569</v>
+      </c>
+      <c r="G4" s="3">
+        <v>64520</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>64520</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="3">
+        <v>7569</v>
+      </c>
+      <c r="G5" s="3">
+        <v>64520</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>64520</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="4">
+        <v>16862</v>
+      </c>
+      <c r="G7" s="4">
+        <v>313</v>
+      </c>
+      <c r="H7" s="4">
+        <v>276177</v>
+      </c>
+      <c r="I7" s="4">
+        <v>276177</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="4">
+        <v>16862</v>
+      </c>
+      <c r="G8" s="4">
+        <v>313</v>
+      </c>
+      <c r="H8" s="4">
+        <v>276177</v>
+      </c>
+      <c r="I8" s="4">
+        <v>276177</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="4">
+        <v>16862</v>
+      </c>
+      <c r="G9" s="4">
+        <v>313</v>
+      </c>
+      <c r="H9" s="4">
+        <v>276177</v>
+      </c>
+      <c r="I9" s="4">
+        <v>276177</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="4">
+        <v>16862</v>
+      </c>
+      <c r="G10" s="4">
+        <v>313</v>
+      </c>
+      <c r="H10" s="4">
+        <v>276177</v>
+      </c>
+      <c r="I10" s="4">
+        <v>276177</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="29">
+        <v>16862</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="15"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="15"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="15"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="15"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="16"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="15"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="15"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="15"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="15"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="16"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EC5171-6C71-CB4F-A265-8AC6225C86D6}">
+  <dimension ref="A1:Z28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="11"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="3">
+        <v>809582</v>
+      </c>
+      <c r="G2" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="L2" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="3">
+        <v>809582</v>
+      </c>
+      <c r="G3" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="3">
+        <v>809582</v>
+      </c>
+      <c r="G4" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="3">
+        <v>809582</v>
+      </c>
+      <c r="G5" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>31026897</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="4">
+        <v>686674</v>
+      </c>
+      <c r="G7" s="4">
+        <v>31853053</v>
+      </c>
+      <c r="H7" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="I7" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="4">
+        <v>686674</v>
+      </c>
+      <c r="G8" s="4">
+        <v>31853053</v>
+      </c>
+      <c r="H8" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="I8" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="4">
+        <v>686674</v>
+      </c>
+      <c r="G9" s="4">
+        <v>31853053</v>
+      </c>
+      <c r="H9" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="I9" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="4">
+        <v>686674</v>
+      </c>
+      <c r="G10" s="4">
+        <v>31853053</v>
+      </c>
+      <c r="H10" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="I10" s="4">
+        <v>177834009</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="15"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="15"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="15"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="15"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="16"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="15"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="15"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="15"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="15"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="16"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF2D920-D934-9E4E-B4DA-19608454C8CE}">
+  <dimension ref="A1:Z28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="11"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="L1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1024972</v>
+      </c>
+      <c r="G2" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="L2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1024972</v>
+      </c>
+      <c r="G3" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="J3" s="15"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1024972</v>
+      </c>
+      <c r="G4" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1024972</v>
+      </c>
+      <c r="G5" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>23372644</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="4">
+        <v>768819</v>
+      </c>
+      <c r="G7" s="4">
+        <v>37830480</v>
+      </c>
+      <c r="H7" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="I7" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="4">
+        <v>768819</v>
+      </c>
+      <c r="G8" s="4">
+        <v>37830480</v>
+      </c>
+      <c r="H8" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="I8" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="4">
+        <v>768819</v>
+      </c>
+      <c r="G9" s="4">
+        <v>37830480</v>
+      </c>
+      <c r="H9" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="I9" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="4">
+        <v>768819</v>
+      </c>
+      <c r="G10" s="4">
+        <v>37830480</v>
+      </c>
+      <c r="H10" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="I10" s="4">
+        <v>153328730</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="29">
+        <v>768819</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="15"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="15"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="15"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="15"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="16"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="15"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="15"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="15"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="15"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="16"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5288F6-690F-014A-8B92-C00F486D51E6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266A1BF3-84D2-DB44-A3F6-007BD91A3ADF}">
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:Z26"/>
     </sheetView>
   </sheetViews>
@@ -5433,7 +8980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F28B05-22D4-AD4F-922C-114B867D4128}">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -6238,7 +9785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF67325-ECCC-DB41-9BA5-513761FF7618}">
   <dimension ref="A1:Z151"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView topLeftCell="A137" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection sqref="A1:I151"/>
     </sheetView>
   </sheetViews>
@@ -16345,8 +19892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBD9969-057A-7E46-B6E2-BFDB8CEC0CA9}">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16621,9 +20168,7 @@
       <c r="I6" s="7">
         <v>916</v>
       </c>
-      <c r="J6" s="28" t="s">
-        <v>53</v>
-      </c>
+      <c r="J6" s="28"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -18569,7 +22114,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18837,7 +22382,7 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="29">
         <v>9204</v>
       </c>
       <c r="G6" s="2">
@@ -19062,7 +22607,7 @@
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="29">
         <v>2787</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -19289,7 +22834,7 @@
       <c r="E16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="29" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -19516,7 +23061,7 @@
       <c r="E21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="29">
         <v>721</v>
       </c>
       <c r="G21" s="2" t="s">

</xml_diff>

<commit_message>
Updated excel for DRUG/ ATC/RXNORM and verification
</commit_message>
<xml_diff>
--- a/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
+++ b/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subracr1/Projects/tanagra/tanagra-workbench/api/db-cdr/generate-cdr/cb-criteria-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323770DD-6938-7C41-B859-67841CA860F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6320EA00-C4F5-3B4D-A06C-093A90087D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37120" yWindow="2620" windowWidth="34660" windowHeight="19080" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="33720" windowHeight="20920" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-ALL" sheetId="24" r:id="rId1"/>
@@ -30,15 +30,16 @@
     <sheet name="14-LOINC-CLIN" sheetId="21" r:id="rId15"/>
     <sheet name="15-LOINC-LABS" sheetId="22" r:id="rId16"/>
     <sheet name="16-MEAS-SNOMED" sheetId="25" r:id="rId17"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="23" r:id="rId19"/>
+    <sheet name="17-DRUGS-RXNORM" sheetId="26" r:id="rId18"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2830" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="176">
   <si>
     <t>run_type</t>
   </si>
@@ -945,6 +946,44 @@
                   from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'MEASUREMENT' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
               )
 order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- DRUG_EXPOSURE - ATC/RXNORM - SQL-ORDER = 17
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'drug-rxnorm-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'DRUG' and type = 'ATC' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'drug-rxnorm-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'DRUG' and type = 'ATC' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'drug-rxnorm-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'DRUG' and type = 'ATC' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'drug-rxnorm-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'DRUG' and type = 'ATC' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'drug-rxnorm-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'DRUG' and type = 'ATC' and is_standard = 1 group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>DRUG</t>
+  </si>
+  <si>
+    <t>ATC</t>
+  </si>
+  <si>
+    <t>drug-rxnorm-name</t>
+  </si>
+  <si>
+    <t>11104956*</t>
   </si>
 </sst>
 </file>
@@ -9923,7 +9962,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:I11"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10764,7 +10803,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L2" sqref="L2:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11465,8 +11504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCCA111-7090-4D44-9A58-B8DAD714D931}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12305,7 +12344,7 @@
   <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+      <selection activeCell="L2" sqref="L2:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13140,19 +13179,711 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5288F6-690F-014A-8B92-C00F486D51E6}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C40265-EB1D-734F-8F85-DF55F9F74613}">
+  <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="9"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="L1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1027</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="I2" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="L2" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1027</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="I3" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1027</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="I4" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1027</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>11104999</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1027</v>
+      </c>
+      <c r="G6" s="21">
+        <v>-43</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J7" s="12"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J8" s="12"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J9" s="12"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J10" s="12"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J11" s="13"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="12"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="12"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="12"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="25"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="12"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="25"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="13"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="12"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="12"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="25"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="12"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
+      <c r="W19" s="25"/>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="25"/>
+      <c r="Z19" s="25"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="12"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="13"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="25"/>
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="25"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
+      <c r="X26" s="25"/>
+      <c r="Y26" s="25"/>
+      <c r="Z26" s="25"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="25"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="25"/>
+      <c r="X28" s="25"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914D1EC-8DC1-CE42-8722-2C2552E9ACC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5288F6-690F-014A-8B92-C00F486D51E6}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13955,11 +14686,23 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914D1EC-8DC1-CE42-8722-2C2552E9ACC7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266A1BF3-84D2-DB44-A3F6-007BD91A3ADF}">
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:Z26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated SQLs, excel-sheet, and verification for PROC-OCCUR-SNOMED-STD
</commit_message>
<xml_diff>
--- a/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
+++ b/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subracr1/Projects/tanagra/tanagra-workbench/api/db-cdr/generate-cdr/cb-criteria-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBA7426-1DE1-9B4A-AE6A-DD2083F093BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D349BCC7-4C97-084D-B441-B424C911A6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="33720" windowHeight="20920" firstSheet="9" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="33720" windowHeight="20920" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-ALL" sheetId="24" r:id="rId1"/>
@@ -32,15 +32,16 @@
     <sheet name="16-MEAS-SNOMED" sheetId="25" r:id="rId17"/>
     <sheet name="17-DRUGS-RXNORM" sheetId="26" r:id="rId18"/>
     <sheet name="18-PROC-OCCUR-SNOMED-SRC" sheetId="27" r:id="rId19"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId20"/>
-    <sheet name="Sheet1" sheetId="23" r:id="rId21"/>
+    <sheet name="19-PROC-OCCUR-SNOMED-STD" sheetId="28" r:id="rId20"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId21"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="186">
   <si>
     <t>run_type</t>
   </si>
@@ -1026,6 +1027,41 @@
   </si>
   <si>
     <t>135076*</t>
+  </si>
+  <si>
+    <t>SQL Snippet:
+-- PROCEDURE_OCCURRENCE - SNOMED - STANDARD - SQL-ORDER = 19
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'proc-occur-snomed-std-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'PROCEDURE' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'proc-occur-snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'PROCEDURE' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'proc-occur-snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'PROCEDURE' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'proc-occur-snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'PROCEDURE' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'proc-occur-snomed-std-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'PROCEDURE' and type = 'SNOMED' and is_standard = 1 group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>proc-occur-snomed-std-name</t>
+  </si>
+  <si>
+    <t>8864280*</t>
+  </si>
+  <si>
+    <t>902677*</t>
   </si>
 </sst>
 </file>
@@ -13928,7 +13964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFCE117F-0B64-6844-B79E-82AC15263FED}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -13938,7 +13974,7 @@
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
@@ -15558,6 +15594,845 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF99C94D-F7B4-FC41-9485-70326B888AB4}">
+  <dimension ref="A1:Z28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="9"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="L1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="3">
+        <v>47625</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="L2" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="3">
+        <v>47625</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="3">
+        <v>47625</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="3">
+        <v>47625</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2242526</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="21">
+        <v>47625</v>
+      </c>
+      <c r="G6" s="21">
+        <v>2242526</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
+        <v>2242526</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="4">
+        <v>52659</v>
+      </c>
+      <c r="G7" s="4">
+        <v>902678</v>
+      </c>
+      <c r="H7" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="I7" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="4">
+        <v>52659</v>
+      </c>
+      <c r="G8" s="4">
+        <v>902678</v>
+      </c>
+      <c r="H8" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="I8" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="4">
+        <v>52659</v>
+      </c>
+      <c r="G9" s="4">
+        <v>902678</v>
+      </c>
+      <c r="H9" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="I9" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="4">
+        <v>52659</v>
+      </c>
+      <c r="G10" s="4">
+        <v>902678</v>
+      </c>
+      <c r="H10" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="I10" s="4">
+        <v>8864281</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="24">
+        <v>52659</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J12" s="12"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J13" s="12"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J14" s="12"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J15" s="12"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="J16" s="13"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+    </row>
+    <row r="17" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J17" s="12"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+    </row>
+    <row r="18" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J18" s="12"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+    </row>
+    <row r="19" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J19" s="12"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+    </row>
+    <row r="20" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J20" s="12"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+    </row>
+    <row r="21" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="J21" s="13"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+    </row>
+    <row r="22" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+    </row>
+    <row r="23" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+    </row>
+    <row r="24" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+    </row>
+    <row r="25" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+    </row>
+    <row r="26" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+    </row>
+    <row r="27" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+    </row>
+    <row r="28" spans="10:26" x14ac:dyDescent="0.2">
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="27"/>
+      <c r="V28" s="27"/>
+      <c r="W28" s="27"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z26"/>
+    <mergeCell ref="L27:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5288F6-690F-014A-8B92-C00F486D51E6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -15569,7 +16444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914D1EC-8DC1-CE42-8722-2C2552E9ACC7}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated SQLs, excel-sheet, and verification for OBSERVATION
</commit_message>
<xml_diff>
--- a/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
+++ b/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subracr1/Projects/tanagra/tanagra-workbench/api/db-cdr/generate-cdr/cb-criteria-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D349BCC7-4C97-084D-B441-B424C911A6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0FA0BE-B6C2-594E-9878-BF8F40C79EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="33720" windowHeight="20920" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="33720" windowHeight="20920" firstSheet="14" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="00-ALL" sheetId="24" r:id="rId1"/>
@@ -33,15 +33,16 @@
     <sheet name="17-DRUGS-RXNORM" sheetId="26" r:id="rId18"/>
     <sheet name="18-PROC-OCCUR-SNOMED-SRC" sheetId="27" r:id="rId19"/>
     <sheet name="19-PROC-OCCUR-SNOMED-STD" sheetId="28" r:id="rId20"/>
-    <sheet name="Sheet14" sheetId="15" r:id="rId21"/>
-    <sheet name="Sheet1" sheetId="23" r:id="rId22"/>
+    <sheet name="20-OBSERVATION" sheetId="29" r:id="rId21"/>
+    <sheet name="Sheet14" sheetId="15" r:id="rId22"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3116" uniqueCount="191">
   <si>
     <t>run_type</t>
   </si>
@@ -1063,6 +1064,44 @@
   <si>
     <t>902677*</t>
   </si>
+  <si>
+    <t>SQL Snippet:
+-- OBSERVATION - SQL-ORDER = 20
+select * from (
+                  select '01-sequential' run_type, domain_id, type, is_group, 'observation-name' name, count(is_group) sum_grp_count
+                       , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySeq.cb_criteria` where domain_id = 'OBSERVATION' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '02-parallel' run_type, domain_id, type, is_group, 'observation-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyPar.cb_criteria` where domain_id = 'OBSERVATION' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '03-parallel-multi' run_type, domain_id, type, is_group, 'observation-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyMult.cb_criteria` where domain_id = 'OBSERVATION' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '10-original' run_type, domain_id, type, is_group, 'observation-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummyOri.cb_criteria` where domain_id = 'OBSERVATION' and is_standard = 1 group by 4,5,3,2
+                  union all
+                  select '20-std-src' run_type, domain_id, type, is_group, 'observation-name' name, count(is_group) sum_grp_count
+                          , sum(item_count) sum_item_count, sum(rollup_count) sum_rollup_count, sum(est_count) sum_est_count
+                  from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria` where domain_id = 'OBSERVATION' and is_standard = 1 group by 4,5,3,2
+              )
+order by domain_id, type, is_group, name, run_type;</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t>observation-name</t>
+  </si>
+  <si>
+    <t>DRG</t>
+  </si>
+  <si>
+    <t>HCPCS</t>
+  </si>
 </sst>
 </file>
 
@@ -15597,8 +15636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF99C94D-F7B4-FC41-9485-70326B888AB4}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16433,6 +16472,1418 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CFD597-B0D0-6646-87A2-2E0396949EF2}">
+  <dimension ref="A1:Z31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="9"/>
+    <col min="12" max="12" width="58.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="L1" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+    </row>
+    <row r="2" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="3">
+        <v>198</v>
+      </c>
+      <c r="G2" s="3">
+        <v>33651</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>33651</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="L2" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="3">
+        <v>198</v>
+      </c>
+      <c r="G3" s="3">
+        <v>33651</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>33651</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="3">
+        <v>198</v>
+      </c>
+      <c r="G4" s="3">
+        <v>33651</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>33651</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="3">
+        <v>198</v>
+      </c>
+      <c r="G5" s="3">
+        <v>33651</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>33651</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="21">
+        <v>198</v>
+      </c>
+      <c r="G6" s="21">
+        <v>33651</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21">
+        <v>33651</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="4">
+        <v>423</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2518</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2518</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="4">
+        <v>423</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2518</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2518</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="4">
+        <v>423</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2518</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2518</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27"/>
+      <c r="Z9" s="27"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="4">
+        <v>423</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2518</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>2518</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="27"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F11" s="24">
+        <v>423</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2518</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2518</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="3">
+        <v>234</v>
+      </c>
+      <c r="G12" s="3">
+        <v>31852</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>31852</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F13" s="3">
+        <v>234</v>
+      </c>
+      <c r="G13" s="3">
+        <v>31852</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>31852</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F14" s="3">
+        <v>234</v>
+      </c>
+      <c r="G14" s="3">
+        <v>31852</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>31852</v>
+      </c>
+      <c r="J14" s="12"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
+      <c r="Z14" s="27"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="3">
+        <v>234</v>
+      </c>
+      <c r="G15" s="3">
+        <v>31852</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>31852</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27"/>
+      <c r="Z15" s="27"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="F16" s="21">
+        <v>234</v>
+      </c>
+      <c r="G16" s="21">
+        <v>31852</v>
+      </c>
+      <c r="H16" s="21">
+        <v>0</v>
+      </c>
+      <c r="I16" s="21">
+        <v>31852</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="4">
+        <v>133</v>
+      </c>
+      <c r="G17" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" s="4">
+        <v>133</v>
+      </c>
+      <c r="G18" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F19" s="4">
+        <v>133</v>
+      </c>
+      <c r="G19" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F20" s="4">
+        <v>133</v>
+      </c>
+      <c r="G20" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>9177609</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F21" s="24">
+        <v>133</v>
+      </c>
+      <c r="G21" s="2">
+        <v>9177609</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>9177609</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27"/>
+      <c r="Z21" s="27"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F22" s="3">
+        <v>755</v>
+      </c>
+      <c r="G22" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="3">
+        <v>755</v>
+      </c>
+      <c r="G23" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="3">
+        <v>755</v>
+      </c>
+      <c r="G24" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="3">
+        <v>755</v>
+      </c>
+      <c r="G25" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>17109880</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="4">
+        <v>2546</v>
+      </c>
+      <c r="G27" s="4">
+        <v>553839</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>553839</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="27"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="27"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2546</v>
+      </c>
+      <c r="G28" s="4">
+        <v>553839</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <v>553839</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2546</v>
+      </c>
+      <c r="G29" s="4">
+        <v>553839</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>553839</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2546</v>
+      </c>
+      <c r="G30" s="4">
+        <v>553839</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>553839</v>
+      </c>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F31" s="24">
+        <v>2546</v>
+      </c>
+      <c r="G31" s="2">
+        <v>553839</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>553839</v>
+      </c>
+      <c r="J31" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z27"/>
+    <mergeCell ref="L28:Z28"/>
+    <mergeCell ref="L29:Z29"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5288F6-690F-014A-8B92-C00F486D51E6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16444,7 +17895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6914D1EC-8DC1-CE42-8722-2C2552E9ACC7}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated to add --batch which ensures no count towards daily quote limits for insert/update to same table.
</commit_message>
<xml_diff>
--- a/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
+++ b/api/db-cdr/generate-cdr/cb-criteria-refactor/verify-counts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/subracr1/Projects/tanagra/tanagra-workbench/api/db-cdr/generate-cdr/cb-criteria-refactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F678F-B628-6443-B8C7-11807812DB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C344125-5FEF-4449-ABFD-40E13445744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="33720" windowHeight="20140" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,14 +22,13 @@
     <sheet name="cb_criteria_attrib" sheetId="39" r:id="rId7"/>
     <sheet name="cb_survey_attrib" sheetId="40" r:id="rId8"/>
     <sheet name="cb_criteria_relationship" sheetId="41" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="37" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2922" uniqueCount="72">
   <si>
     <t>run_type</t>
   </si>
@@ -385,13 +384,7 @@
     <t>1604766</t>
   </si>
   <si>
-    <t>3209532</t>
-  </si>
-  <si>
     <t>11412609616999.221957463765463808</t>
-  </si>
-  <si>
-    <t>22825219233998.443914927530927616</t>
   </si>
   <si>
     <t>SQL Snippet
@@ -420,9 +413,6 @@
                   from `all-of-us-ehr-dev.ChenchalDummySrc.cb_criteria_attribute`group by 3
               )
 order by type, run_type;</t>
-  </si>
-  <si>
-    <t>cb_survey_attribute</t>
   </si>
   <si>
     <t>SQL Snippet
@@ -638,7 +628,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -842,12 +832,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA8186"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -983,9 +967,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1035,7 +1017,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1061,13 +1043,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,19 +1070,20 @@
     <xf numFmtId="49" fontId="18" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1469,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43E1F31-484A-0D48-900A-F46D809B8E62}">
   <dimension ref="A1:L311"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="L235" sqref="L235"/>
+    <sheetView topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="L435" sqref="L435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1545,7 +1522,7 @@
       <c r="I2" s="3">
         <v>769</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="20" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1577,7 +1554,7 @@
       <c r="I3" s="3">
         <v>769</v>
       </c>
-      <c r="L3" s="9"/>
+      <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1607,7 +1584,7 @@
       <c r="I4" s="3">
         <v>769</v>
       </c>
-      <c r="L4" s="9"/>
+      <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1637,7 +1614,7 @@
       <c r="I5" s="3">
         <v>769</v>
       </c>
-      <c r="L5" s="9"/>
+      <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -1667,7 +1644,7 @@
       <c r="I6" s="6">
         <v>769</v>
       </c>
-      <c r="L6" s="9"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1697,7 +1674,7 @@
       <c r="I7" s="4">
         <v>2695033</v>
       </c>
-      <c r="L7" s="9"/>
+      <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -1727,7 +1704,7 @@
       <c r="I8" s="4">
         <v>2695033</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1757,7 +1734,7 @@
       <c r="I9" s="4">
         <v>2695033</v>
       </c>
-      <c r="L9" s="9"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1787,7 +1764,7 @@
       <c r="I10" s="4">
         <v>2695033</v>
       </c>
-      <c r="L10" s="9"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1817,7 +1794,7 @@
       <c r="I11" s="2">
         <v>2695033</v>
       </c>
-      <c r="L11" s="9"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1847,7 +1824,7 @@
       <c r="I12" s="3">
         <v>4955215</v>
       </c>
-      <c r="L12" s="9"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -1877,7 +1854,7 @@
       <c r="I13" s="3">
         <v>4955215</v>
       </c>
-      <c r="L13" s="9"/>
+      <c r="L13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1907,7 +1884,7 @@
       <c r="I14" s="3">
         <v>4955215</v>
       </c>
-      <c r="L14" s="9"/>
+      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1937,7 +1914,7 @@
       <c r="I15" s="3">
         <v>4955215</v>
       </c>
-      <c r="L15" s="9"/>
+      <c r="L15" s="20"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1967,7 +1944,7 @@
       <c r="I16" s="6">
         <v>4955215</v>
       </c>
-      <c r="L16" s="9"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -1997,7 +1974,7 @@
       <c r="I17" s="4">
         <v>2062703</v>
       </c>
-      <c r="L17" s="9"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -2027,7 +2004,7 @@
       <c r="I18" s="4">
         <v>2062703</v>
       </c>
-      <c r="L18" s="9"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -2057,7 +2034,7 @@
       <c r="I19" s="4">
         <v>2062703</v>
       </c>
-      <c r="L19" s="9"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -2087,7 +2064,7 @@
       <c r="I20" s="4">
         <v>2062703</v>
       </c>
-      <c r="L20" s="9"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -2117,7 +2094,7 @@
       <c r="I21" s="2">
         <v>2062703</v>
       </c>
-      <c r="L21" s="9"/>
+      <c r="L21" s="20"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -2147,7 +2124,7 @@
       <c r="I22" s="3">
         <v>2890678</v>
       </c>
-      <c r="L22" s="9"/>
+      <c r="L22" s="20"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -2177,7 +2154,7 @@
       <c r="I23" s="3">
         <v>2890678</v>
       </c>
-      <c r="L23" s="9"/>
+      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -2207,7 +2184,7 @@
       <c r="I24" s="3">
         <v>2890678</v>
       </c>
-      <c r="L24" s="9"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -2237,7 +2214,7 @@
       <c r="I25" s="3">
         <v>2890678</v>
       </c>
-      <c r="L25" s="9"/>
+      <c r="L25" s="20"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -2267,7 +2244,7 @@
       <c r="I26" s="6">
         <v>2890678</v>
       </c>
-      <c r="L26" s="9"/>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
@@ -2297,7 +2274,7 @@
       <c r="I27" s="4">
         <v>1</v>
       </c>
-      <c r="L27" s="9"/>
+      <c r="L27" s="20"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -3824,16 +3801,16 @@
         <v>0</v>
       </c>
       <c r="F80" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" s="4">
-        <v>182</v>
+        <v>91</v>
       </c>
       <c r="H80" s="4">
         <v>0</v>
       </c>
       <c r="I80" s="4">
-        <v>182</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3969,16 +3946,16 @@
         <v>0</v>
       </c>
       <c r="F85" s="3">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="G85" s="3">
-        <v>199070</v>
+        <v>99535</v>
       </c>
       <c r="H85" s="3">
         <v>0</v>
       </c>
       <c r="I85" s="3">
-        <v>199070</v>
+        <v>99535</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -4114,16 +4091,16 @@
         <v>0</v>
       </c>
       <c r="F90" s="4">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="G90" s="4">
-        <v>2906</v>
+        <v>1453</v>
       </c>
       <c r="H90" s="4">
         <v>0</v>
       </c>
       <c r="I90" s="4">
-        <v>2906</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -4404,16 +4381,16 @@
         <v>0</v>
       </c>
       <c r="F100" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G100" s="4">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="H100" s="4">
         <v>0</v>
       </c>
       <c r="I100" s="4">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -6157,31 +6134,31 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" s="12" t="s">
+      <c r="A161" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B161" s="12" t="s">
+      <c r="B161" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C161" s="12" t="s">
+      <c r="C161" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D161" s="12" t="s">
+      <c r="D161" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E161" s="12" t="s">
+      <c r="E161" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F161" s="12" t="s">
+      <c r="F161" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G161" s="12" t="s">
+      <c r="G161" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H161" s="12" t="s">
+      <c r="H161" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I161" s="12" t="s">
+      <c r="I161" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -7973,16 +7950,16 @@
       <c r="F223" s="3">
         <v>2592</v>
       </c>
-      <c r="G223" s="13">
-        <v>0</v>
-      </c>
-      <c r="H223" s="13">
+      <c r="G223" s="11">
+        <v>0</v>
+      </c>
+      <c r="H223" s="11">
         <v>2415916</v>
       </c>
       <c r="I223" s="3">
         <v>2415908</v>
       </c>
-      <c r="J223" s="14" t="s">
+      <c r="J223" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -8005,16 +7982,16 @@
       <c r="F224" s="3">
         <v>2592</v>
       </c>
-      <c r="G224" s="13">
-        <v>0</v>
-      </c>
-      <c r="H224" s="13">
+      <c r="G224" s="11">
+        <v>0</v>
+      </c>
+      <c r="H224" s="11">
         <v>2415916</v>
       </c>
       <c r="I224" s="3">
         <v>2415908</v>
       </c>
-      <c r="J224" s="14" t="s">
+      <c r="J224" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -10549,38 +10526,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBA8600-B746-7245-8571-3B05961C15C3}">
-  <dimension ref="A161:I161"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L318" sqref="L318"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A161" s="11"/>
-      <c r="B161" s="11"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="11"/>
-      <c r="E161" s="11"/>
-      <c r="F161" s="11"/>
-      <c r="G161" s="11"/>
-      <c r="H161" s="11"/>
-      <c r="I161" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BE368B-AA06-E544-893B-EA69A9D143E9}">
   <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H1:H27"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="H260" sqref="H260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10628,7 +10579,7 @@
       <c r="E2" s="3">
         <v>88</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -10648,7 +10599,7 @@
       <c r="E3" s="3">
         <v>88</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -10666,7 +10617,7 @@
       <c r="E4" s="3">
         <v>88</v>
       </c>
-      <c r="H4" s="9"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -10684,7 +10635,7 @@
       <c r="E5" s="3">
         <v>88</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -10702,7 +10653,7 @@
       <c r="E6" s="6">
         <v>88</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -10720,7 +10671,7 @@
       <c r="E7" s="4">
         <v>20187</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -10738,7 +10689,7 @@
       <c r="E8" s="4">
         <v>20187</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -10756,7 +10707,7 @@
       <c r="E9" s="4">
         <v>20187</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -10774,7 +10725,7 @@
       <c r="E10" s="4">
         <v>20187</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -10792,7 +10743,7 @@
       <c r="E11" s="2">
         <v>20187</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -10810,7 +10761,7 @@
       <c r="E12" s="3">
         <v>11776</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -10828,7 +10779,7 @@
       <c r="E13" s="3">
         <v>11776</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -10846,7 +10797,7 @@
       <c r="E14" s="3">
         <v>11776</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -10864,7 +10815,7 @@
       <c r="E15" s="3">
         <v>11776</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -10882,7 +10833,7 @@
       <c r="E16" s="6">
         <v>11776</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -10900,7 +10851,7 @@
       <c r="E17" s="4">
         <v>9204</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -10918,7 +10869,7 @@
       <c r="E18" s="4">
         <v>9204</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -10936,7 +10887,7 @@
       <c r="E19" s="4">
         <v>9204</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -10954,7 +10905,7 @@
       <c r="E20" s="4">
         <v>9204</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -10972,7 +10923,7 @@
       <c r="E21" s="2">
         <v>9204</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -10990,7 +10941,7 @@
       <c r="E22" s="3">
         <v>2787</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="20"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -11008,7 +10959,7 @@
       <c r="E23" s="3">
         <v>2787</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -11026,7 +10977,7 @@
       <c r="E24" s="3">
         <v>2787</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -11044,7 +10995,7 @@
       <c r="E25" s="3">
         <v>2787</v>
       </c>
-      <c r="H25" s="9"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -11062,7 +11013,7 @@
       <c r="E26" s="6">
         <v>2787</v>
       </c>
-      <c r="H26" s="9"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
@@ -11080,7 +11031,7 @@
       <c r="E27" s="4">
         <v>2</v>
       </c>
-      <c r="H27" s="9"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -11725,7 +11676,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -11810,7 +11761,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="4">
-        <v>256</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -11895,7 +11846,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="3">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -12065,7 +12016,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -15157,8 +15108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3630E6-9FEA-CB4F-A0E0-116A3D378D8F}">
   <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G27"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="G205" sqref="G205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15172,16 +15123,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -15201,7 +15152,7 @@
       <c r="D2" s="3">
         <v>88</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -15218,7 +15169,7 @@
       <c r="D3" s="3">
         <v>88</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -15233,7 +15184,7 @@
       <c r="D4" s="3">
         <v>88</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -15248,7 +15199,7 @@
       <c r="D5" s="3">
         <v>88</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -15263,7 +15214,7 @@
       <c r="D6" s="6">
         <v>88</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -15278,7 +15229,7 @@
       <c r="D7" s="4">
         <v>31963</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -15293,7 +15244,7 @@
       <c r="D8" s="4">
         <v>31963</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -15308,7 +15259,7 @@
       <c r="D9" s="4">
         <v>31963</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -15323,7 +15274,7 @@
       <c r="D10" s="4">
         <v>31963</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -15338,7 +15289,7 @@
       <c r="D11" s="2">
         <v>31963</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -15353,7 +15304,7 @@
       <c r="D12" s="3">
         <v>11991</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -15368,7 +15319,7 @@
       <c r="D13" s="3">
         <v>11991</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -15383,7 +15334,7 @@
       <c r="D14" s="3">
         <v>11991</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -15398,7 +15349,7 @@
       <c r="D15" s="3">
         <v>11991</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -15413,7 +15364,7 @@
       <c r="D16" s="6">
         <v>11991</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -15428,7 +15379,7 @@
       <c r="D17" s="4">
         <v>2</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -15443,7 +15394,7 @@
       <c r="D18" s="4">
         <v>2</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -15458,7 +15409,7 @@
       <c r="D19" s="4">
         <v>2</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -15473,7 +15424,7 @@
       <c r="D20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -15488,7 +15439,7 @@
       <c r="D21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -15503,7 +15454,7 @@
       <c r="D22" s="3">
         <v>1</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -15518,7 +15469,7 @@
       <c r="D23" s="3">
         <v>1</v>
       </c>
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -15533,7 +15484,7 @@
       <c r="D24" s="3">
         <v>1</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -15548,7 +15499,7 @@
       <c r="D25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -15563,7 +15514,7 @@
       <c r="D26" s="6">
         <v>1</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
@@ -15578,7 +15529,7 @@
       <c r="D27" s="4">
         <v>2</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -15899,7 +15850,7 @@
         <v>38</v>
       </c>
       <c r="D50" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -15969,7 +15920,7 @@
         <v>38</v>
       </c>
       <c r="D55" s="3">
-        <v>256</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -16039,7 +15990,7 @@
         <v>38</v>
       </c>
       <c r="D60" s="4">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -16179,7 +16130,7 @@
         <v>38</v>
       </c>
       <c r="D70" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -16898,7 +16849,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>35</v>
@@ -18168,8 +18119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0067027-22C4-D647-B2DB-EFF5F1ABD342}">
   <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection sqref="A1:C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18181,13 +18132,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -18204,7 +18155,7 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -18218,7 +18169,7 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -18230,7 +18181,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -18242,7 +18193,7 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -18254,7 +18205,7 @@
       <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -18266,7 +18217,7 @@
       <c r="C7" s="4">
         <v>1027</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -18278,7 +18229,7 @@
       <c r="C8" s="4">
         <v>1027</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -18290,7 +18241,7 @@
       <c r="C9" s="4">
         <v>1027</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -18302,7 +18253,7 @@
       <c r="C10" s="4">
         <v>1027</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -18314,7 +18265,7 @@
       <c r="C11" s="2">
         <v>1027</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -18326,7 +18277,7 @@
       <c r="C12" s="3">
         <v>63848</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -18338,7 +18289,7 @@
       <c r="C13" s="3">
         <v>63848</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -18350,7 +18301,7 @@
       <c r="C14" s="3">
         <v>63848</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -18362,7 +18313,7 @@
       <c r="C15" s="3">
         <v>63848</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -18374,7 +18325,7 @@
       <c r="C16" s="6">
         <v>63848</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -18386,7 +18337,7 @@
       <c r="C17" s="4">
         <v>90</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
@@ -18398,7 +18349,7 @@
       <c r="C18" s="4">
         <v>90</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -18410,7 +18361,7 @@
       <c r="C19" s="4">
         <v>90</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -18422,7 +18373,7 @@
       <c r="C20" s="4">
         <v>90</v>
       </c>
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -18434,7 +18385,7 @@
       <c r="C21" s="2">
         <v>90</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -18446,7 +18397,7 @@
       <c r="C22" s="3">
         <v>15570</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -18458,7 +18409,7 @@
       <c r="C23" s="3">
         <v>15570</v>
       </c>
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -18470,7 +18421,7 @@
       <c r="C24" s="3">
         <v>15570</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -18480,9 +18431,9 @@
         <v>16</v>
       </c>
       <c r="C25" s="3">
-        <v>15571</v>
-      </c>
-      <c r="G25" s="9"/>
+        <v>15570</v>
+      </c>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -18494,7 +18445,7 @@
       <c r="C26" s="6">
         <v>15570</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
@@ -18506,7 +18457,7 @@
       <c r="C27" s="4">
         <v>128</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -18538,7 +18489,7 @@
         <v>46</v>
       </c>
       <c r="C30" s="4">
-        <v>256</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -18868,7 +18819,7 @@
         <v>42</v>
       </c>
       <c r="C60" s="4">
-        <v>762</v>
+        <v>739</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -19528,7 +19479,7 @@
         <v>51</v>
       </c>
       <c r="C120" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -19774,8 +19725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96631CF9-4D7F-424C-8FFF-D68FE029309A}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19787,13 +19738,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -19824,7 +19775,7 @@
       <c r="C2" s="3">
         <v>3334231</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H2" s="8"/>
@@ -19852,7 +19803,7 @@
       <c r="C3" s="3">
         <v>3334231</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -19878,7 +19829,7 @@
       <c r="C4" s="3">
         <v>3334231</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -19904,7 +19855,7 @@
       <c r="C5" s="3">
         <v>3334231</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -19930,7 +19881,7 @@
       <c r="C6" s="6">
         <v>3334231</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -19956,7 +19907,7 @@
       <c r="C7" s="4">
         <v>68312</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -19982,7 +19933,7 @@
       <c r="C8" s="4">
         <v>68312</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -20008,7 +19959,7 @@
       <c r="C9" s="4">
         <v>68312</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -20032,9 +19983,9 @@
         <v>38</v>
       </c>
       <c r="C10" s="4">
-        <v>68467</v>
-      </c>
-      <c r="G10" s="9"/>
+        <v>68312</v>
+      </c>
+      <c r="G10" s="20"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -20060,7 +20011,7 @@
       <c r="C11" s="2">
         <v>68312</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -20086,7 +20037,7 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -20112,7 +20063,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -20138,7 +20089,7 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -20164,7 +20115,7 @@
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -20190,7 +20141,7 @@
       <c r="C16" s="6">
         <v>1</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -20216,7 +20167,7 @@
       <c r="C17" s="4">
         <v>38450</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -20242,7 +20193,7 @@
       <c r="C18" s="4">
         <v>38450</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -20268,7 +20219,7 @@
       <c r="C19" s="4">
         <v>38450</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -20294,7 +20245,7 @@
       <c r="C20" s="4">
         <v>38450</v>
       </c>
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -20320,7 +20271,7 @@
       <c r="C21" s="2">
         <v>38450</v>
       </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -20346,7 +20297,7 @@
       <c r="C22" s="3">
         <v>4289</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -20372,7 +20323,7 @@
       <c r="C23" s="3">
         <v>4289</v>
       </c>
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -20398,7 +20349,7 @@
       <c r="C24" s="3">
         <v>4289</v>
       </c>
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -20424,7 +20375,7 @@
       <c r="C25" s="3">
         <v>4289</v>
       </c>
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -20450,7 +20401,7 @@
       <c r="C26" s="6">
         <v>3534</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
@@ -20462,7 +20413,7 @@
       <c r="C27" s="4">
         <v>23</v>
       </c>
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -20851,7 +20802,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20863,13 +20814,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -20900,7 +20851,7 @@
       <c r="C2" s="3">
         <v>24976</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="20" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="8"/>
@@ -20928,7 +20879,7 @@
       <c r="C3" s="3">
         <v>24976</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -20954,7 +20905,7 @@
       <c r="C4" s="3">
         <v>24976</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -20980,7 +20931,7 @@
       <c r="C5" s="3">
         <v>24976</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -21006,7 +20957,7 @@
       <c r="C6" s="6">
         <v>24976</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -21023,7 +20974,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G7" s="9"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -21040,7 +20991,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G8" s="9"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -21057,7 +21008,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G9" s="9"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -21074,7 +21025,7 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G10" s="9"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -21091,7 +21042,7 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G11" s="9"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -21108,7 +21059,7 @@
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -21125,7 +21076,7 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -21142,7 +21093,7 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -21159,7 +21110,7 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -21176,7 +21127,7 @@
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -21193,7 +21144,7 @@
       <c r="U16" s="8"/>
     </row>
     <row r="17" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -21210,7 +21161,7 @@
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -21227,7 +21178,7 @@
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -21244,7 +21195,7 @@
       <c r="U19" s="8"/>
     </row>
     <row r="20" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -21261,7 +21212,7 @@
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -21278,7 +21229,7 @@
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -21295,7 +21246,7 @@
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -21312,7 +21263,7 @@
       <c r="U23" s="8"/>
     </row>
     <row r="24" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -21329,7 +21280,7 @@
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -21346,10 +21297,10 @@
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21364,7 +21315,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21377,16 +21328,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -21417,10 +21368,10 @@
       <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="20" t="s">
         <v>66</v>
       </c>
       <c r="H2" s="8"/>
@@ -21448,10 +21399,10 @@
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -21477,10 +21428,10 @@
       <c r="C4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -21506,10 +21457,10 @@
       <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="9"/>
+      <c r="D5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -21535,10 +21486,10 @@
       <c r="C6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -21564,10 +21515,10 @@
       <c r="C7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="9"/>
+      <c r="D7" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -21593,10 +21544,10 @@
       <c r="C8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="9"/>
+      <c r="D8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="20"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -21622,10 +21573,10 @@
       <c r="C9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="9"/>
+      <c r="D9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="20"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -21651,13 +21602,11 @@
       <c r="C10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="9"/>
+      <c r="D10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -21683,10 +21632,10 @@
       <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="9"/>
+      <c r="D11" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="20"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -21703,7 +21652,7 @@
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -21720,7 +21669,7 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -21737,7 +21686,7 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -21754,7 +21703,7 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -21771,7 +21720,7 @@
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -21788,7 +21737,7 @@
       <c r="U16" s="8"/>
     </row>
     <row r="17" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -21805,7 +21754,7 @@
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -21822,7 +21771,7 @@
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -21839,7 +21788,7 @@
       <c r="U19" s="8"/>
     </row>
     <row r="20" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -21856,7 +21805,7 @@
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -21873,7 +21822,7 @@
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -21890,7 +21839,7 @@
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -21907,7 +21856,7 @@
       <c r="U23" s="8"/>
     </row>
     <row r="24" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -21924,7 +21873,7 @@
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -21941,10 +21890,10 @@
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -21959,7 +21908,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21972,16 +21921,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -22007,16 +21956,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>71</v>
+      <c r="G2" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -22038,15 +21987,15 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -22067,15 +22016,15 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -22096,18 +22045,17 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9"/>
+      <c r="D5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -22128,16 +22076,17 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -22158,16 +22107,17 @@
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="G7" s="9"/>
+      <c r="D7" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -22188,16 +22138,17 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="G8" s="9"/>
+      <c r="D8" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -22218,16 +22169,17 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="G9" s="9"/>
+      <c r="D9" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -22248,18 +22200,17 @@
         <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="9"/>
+      <c r="D10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -22280,15 +22231,15 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="9"/>
+      <c r="D11" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="20"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -22305,7 +22256,7 @@
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -22322,7 +22273,7 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -22339,7 +22290,7 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -22356,7 +22307,7 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -22373,7 +22324,7 @@
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -22390,7 +22341,7 @@
       <c r="U16" s="8"/>
     </row>
     <row r="17" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -22407,7 +22358,7 @@
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -22424,7 +22375,7 @@
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -22441,8 +22392,8 @@
       <c r="U19" s="8"/>
     </row>
     <row r="20" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D20" s="21"/>
-      <c r="G20" s="9"/>
+      <c r="D20" s="18"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -22459,7 +22410,7 @@
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -22476,7 +22427,7 @@
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -22493,7 +22444,7 @@
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -22510,7 +22461,7 @@
       <c r="U23" s="8"/>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -22527,7 +22478,7 @@
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -22544,10 +22495,10 @@
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -22562,7 +22513,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22574,13 +22525,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -22606,13 +22557,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" s="3">
         <v>233788</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>73</v>
+      <c r="G2" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -22634,12 +22585,12 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3">
         <v>233788</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -22660,12 +22611,12 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3">
         <v>233788</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -22686,12 +22637,12 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="3">
-        <v>467576</v>
-      </c>
-      <c r="G5" s="9"/>
+        <v>233788</v>
+      </c>
+      <c r="G5" s="20"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -22712,12 +22663,12 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6">
         <v>233788</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -22734,7 +22685,7 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G7" s="9"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -22751,7 +22702,7 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G8" s="9"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -22768,7 +22719,7 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G9" s="9"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -22785,7 +22736,7 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G10" s="9"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -22802,7 +22753,7 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G11" s="9"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -22819,7 +22770,7 @@
       <c r="U11" s="8"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G12" s="9"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -22836,7 +22787,7 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G13" s="9"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -22853,7 +22804,7 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G14" s="9"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -22870,7 +22821,7 @@
       <c r="U14" s="8"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G15" s="9"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -22887,7 +22838,7 @@
       <c r="U15" s="8"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="G16" s="9"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -22904,7 +22855,7 @@
       <c r="U16" s="8"/>
     </row>
     <row r="17" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G17" s="9"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -22921,7 +22872,7 @@
       <c r="U17" s="8"/>
     </row>
     <row r="18" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G18" s="9"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -22938,7 +22889,7 @@
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G19" s="9"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -22955,7 +22906,7 @@
       <c r="U19" s="8"/>
     </row>
     <row r="20" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G20" s="9"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -22972,7 +22923,7 @@
       <c r="U20" s="8"/>
     </row>
     <row r="21" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G21" s="9"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -22989,7 +22940,7 @@
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G22" s="9"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -23006,7 +22957,7 @@
       <c r="U22" s="8"/>
     </row>
     <row r="23" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G23" s="9"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -23023,7 +22974,7 @@
       <c r="U23" s="8"/>
     </row>
     <row r="24" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G24" s="9"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -23040,7 +22991,7 @@
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G25" s="9"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -23057,10 +23008,10 @@
       <c r="U25" s="8"/>
     </row>
     <row r="26" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G26" s="9"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G27" s="9"/>
+      <c r="G27" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>